<commit_message>
20150113 +++++++ cs-厂商 end
</commit_message>
<xml_diff>
--- a/页面对照表.xlsx
+++ b/页面对照表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>常见问题.psd</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,15 +80,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>搜索列表 - 大图版面.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>search-list-b.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>search-class.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索列表.psd,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索列表 - 大图版面.psd,搜索列表 - 排序.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search-list.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -489,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -534,10 +542,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20150113 +++++++ cs-厂商 end +
</commit_message>
<xml_diff>
--- a/页面对照表.xlsx
+++ b/页面对照表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>常见问题.psd</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -28,75 +28,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>shop-index.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类搜索2.psd,分类搜索2 - 展开.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于我们.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>about-us.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联系我们.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contact-us.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>品牌介绍.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>introduce.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品-评论详情-更多.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment-list.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品详情 - 2.psd,商品详情 - 2 - 弹出规格.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-show.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search-list-b.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search-class.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索列表.psd,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索列表 - 大图版面.psd,搜索列表 - 排序.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search-list.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>店铺首页.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>cs-厂商</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>shop-index.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分类搜索2.psd,分类搜索2 - 展开.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关于我们.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>about-us.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>联系我们.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>contact-us.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>品牌介绍.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>introduce.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品-评论详情-更多.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comment-list.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品详情 - 2.psd,商品详情 - 2 - 弹出规格.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shop-show.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>search-list-b.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>search-class.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索列表.psd,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索列表 - 大图版面.psd,搜索列表 - 排序.psd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>search-list.html</t>
+    <t>mj-买家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>店铺首页-搜索.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-index-mj.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-index-mj-search.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品详情 - 2.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shop-show-mj.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +150,15 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -149,9 +186,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -473,7 +513,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
@@ -489,71 +529,100 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20150113 +++++++ cs-厂商 end ++ end
</commit_message>
<xml_diff>
--- a/页面对照表.xlsx
+++ b/页面对照表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>常见问题.psd</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,22 @@
   </si>
   <si>
     <t>shop-show-mj.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的订单3.psd,我的订单3 - 下拉.psd,我的订单-待发货.psd,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的订单-待发货-订单详情 - 申请退款.psd,我的订单-待发货-订单详情 - 退款成功.psd,我的订单-待发货-订单详情.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my-indent.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my-indent-dfh.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -186,13 +202,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -625,6 +644,22 @@
         <v>27</v>
       </c>
     </row>
+    <row r="20" spans="1:2" ht="27" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20150116++++++ fix footerweidai +
</commit_message>
<xml_diff>
--- a/页面对照表.xlsx
+++ b/页面对照表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>常见问题.psd</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,6 +449,38 @@
   </si>
   <si>
     <t>news-show.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我的收入 - 2.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入明细.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income-detail.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入明细-详情页面.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收入明细-详情页面个人明细和扩展团队.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income-detail-info.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>income-detail-info2.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -842,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1292,6 +1324,38 @@
         <v>108</v>
       </c>
     </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20150116++++++ fix footerweidai + end
</commit_message>
<xml_diff>
--- a/页面对照表.xlsx
+++ b/页面对照表.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>常见问题.psd</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -481,6 +481,14 @@
   </si>
   <si>
     <t>income-detail-info2.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队管理.psd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>team-management.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -874,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1356,6 +1364,14 @@
         <v>116</v>
       </c>
     </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>117</v>
+      </c>
+      <c r="B88" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>